<commit_message>
Suplies filtering by products with report
</commit_message>
<xml_diff>
--- a/Mushka.Infrastructure.Excel/templates/export_supply_products_template.xlsx
+++ b/Mushka.Infrastructure.Excel/templates/export_supply_products_template.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MUSHKA\mushka-accounting\Mushka.Infrastructure.Excel\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Mine\MUSHKA\accounting\Mushka.Infrastructure.Excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25245" windowHeight="8685"/>
   </bookViews>
   <sheets>
-    <sheet name="Носки" sheetId="1" r:id="rId1"/>
+    <sheet name="Поступления" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
@@ -24,16 +24,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Список поступлений товаров</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Список поступлений товаров в разрезе поступлений</t>
+  </si>
+  <si>
+    <t>Товар</t>
+  </si>
+  <si>
+    <t>№</t>
+  </si>
+  <si>
+    <t>Поставщик</t>
+  </si>
+  <si>
+    <t>Дата
+поступления</t>
+  </si>
+  <si>
+    <t>Цена
+за единицу</t>
+  </si>
+  <si>
+    <t>Количество
+в поставке</t>
+  </si>
+  <si>
+    <t>На сумму</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +82,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -67,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -75,11 +107,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -87,12 +143,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -374,54 +441,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H7"/>
+  <dimension ref="A2:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="8" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="2"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="2"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+    <row r="7" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="3"/>
     </row>
+    <row r="8" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:G2"/>
+  <mergeCells count="2">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>